<commit_message>
Python Data cleaning project
RealEstate files uploaded
</commit_message>
<xml_diff>
--- a/Binomial Distribution Assignment.xlsx
+++ b/Binomial Distribution Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2a1a4fdcfee177c1/Documents/GitHub/Data-Science-Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{3ED8D7F3-7718-4463-9590-3CD2EC994FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9533594-06A1-4808-A972-A3F4DD215022}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{3ED8D7F3-7718-4463-9590-3CD2EC994FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E863B158-FEC6-40D1-845A-827C46D9DA14}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B16C8813-0A5C-40D6-AFA7-16F7A6832052}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Find the probability of whether a child prefers a cat or dog</t>
   </si>
@@ -59,6 +59,21 @@
   </si>
   <si>
     <t>Binomial Dist:</t>
+  </si>
+  <si>
+    <t>probability dog</t>
+  </si>
+  <si>
+    <t>probability cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factorial </t>
+  </si>
+  <si>
+    <t>equation=probability dog ^dog outcome * probability cat^ cat outcome *( (total factorial)/(dog factorial * cat factorial))</t>
+  </si>
+  <si>
+    <t>Binomial distribution = probability that another set of 10 kids would prefer dogs</t>
   </si>
 </sst>
 </file>
@@ -117,10 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,28 +451,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC8FFF6-DECC-40FB-A3B3-AB8F693761A9}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -464,23 +483,44 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f>D3^D6</f>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="J6">
+        <f>D4^D7</f>
+        <v>0.125</v>
+      </c>
+      <c r="L6">
+        <f>FACT(D5)/(FACT(D6)*FACT(D7))</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -489,19 +529,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="3">
+        <f>H6*J6*L6</f>
+        <v>0.1171875</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2">
-        <f>_xlfn.BINOM.DIST(D6,D5,D3,TRUE)</f>
-        <v>0.9453125</v>
+        <f>_xlfn.BINOM.DIST(D6,D5,D3,FALSE)</f>
+        <v>0.11718750000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>